<commit_message>
added script and file to find alternative treatment chosen given all alternatives,treatments, and sizes
Former-commit-id: 512ecbb2118201a226e328b74962bafbad79f919
</commit_message>
<xml_diff>
--- a/src/derivation/python/data/bluebook_manual_data_online.xlsx
+++ b/src/derivation/python/data/bluebook_manual_data_online.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_290e\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2cfd\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A461718E-3449-4D99-B82C-5E3A5F63F0A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{550CC430-8B60-4812-AFFF-1F1BE7CA67B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2868" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="1037">
   <si>
     <t>start_date</t>
   </si>
@@ -2538,6 +2538,9 @@
     <t>(11) The 25 basis point tightening of Alternative C might be favored if the Committee wanted to lean against the inflationary bias that may well be inherent in the current and prospective tautness of labor markets.</t>
   </si>
   <si>
+    <t>sufficient chances of a shortfall in activity from the staff forecast to suggest a small easing at this time-</t>
+  </si>
+  <si>
     <t>The dollar would be expected to trade around its levels of late, off some from its recent peak (23) The Committee may see sufficient chances of a shortfall in activity from the staff forecast to suggest a small easing at this time--as in the 25 basis point decline in the federal funds rate under alternative A.</t>
   </si>
   <si>
@@ -2547,6 +2550,9 @@
     <t>(24) Alternative C might be favored if the Committee saw the economy as continuing to operate beyond its potential, with the risk that sustained pressures on labor markets might show through more forcefully than in the staff forecast to higher labor costs and prices, perhaps hinted at in the recent employment cost report.</t>
   </si>
   <si>
+    <t>25 basis point reduction in the federal funds rate under alternative A would translate to nearly comparable reductions in other short-term rates.</t>
+  </si>
+  <si>
     <t>(10) If the Committee saw substantial risks of a significantly weaker economy than in the staff forecast, it might want to move promptly to ease policy, perhaps by lowering the federal funds rate 1/4 percentage point, as in alternative A. (11) The 25 basis point reduction in the federal funds rate under alternative A would translate to nearly comparable reductions in other short-term rates.</t>
   </si>
   <si>
@@ -2556,6 +2562,9 @@
     <t>(12) Alternative C would tend to be favored to the extent that the Committee saw the risks as more heavily weighted toward a pickup in inflation. (13) Short-term rates would rise by the full amount of the 25 basis point tightening of policy under alternative C, which is unanticipated in the market.</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>(8) If the Committee views the Greenbook forecast as both likely and acceptable, it might be inclined to maintain its current 5-1/2 percent intended federal funds rate, as under alternative B. Although that forecast has an underlying upward tilt to inflation in 1999 as -8- labor markets remain quite tight, that tilt is gradual and starts from a lower inflation rate in 1998 than the Committee had anticipated only a few months ago, judging from the central tendencies of members' CPI projections in February. 2 Even if the Committee were troubled by the underlying uptrend of inflation in the staff forecast, it might still be willing to adopt the unchanged federal funds rate of alternative B. (13) Under the stable money market conditions of alternative B, the staffs projected 2-1/2 percentage point moderation in the pace of nominal GDP from the first to the third quarter of this year should be associated with a noticeable slowdown in the expansion of the debt and monetary aggregates. (14) Under alternative B, M2 growth is expected to slow significantly to a 3 percent average rate over the April-to-September period, with a little more than 1 percentage point of the slowdown from the first four months of 1998 representing the projected unwinding of the previous artificial boost related to special tax and mortgage-refinancing factors. (15) Projected M3 growth under alternative B would dip to a 5-1/2 percent rate from April through September, reflecting some expected reduction in the growth of depository funding needs associated with the anticipated marked slowing in depository credit expansion - 13 - over that interval.</t>
   </si>
   <si>
@@ -2577,18 +2586,27 @@
     <t>In either case, it may prefer to apply additional monetary restraint at this meeting, as in the 25 basis point increase in the federal funds rate of alternative C. (9) Markets would be somewhat unsettled by the 25 basis point firming action of alternative C at this meeting, which would come as a surprise.</t>
   </si>
   <si>
+    <t>the weaker outlook for the U.S. economy</t>
+  </si>
+  <si>
     <t>3 (7) To begin addressing the weaker outlook for the U.S. economy, the Committee may wish to reduce the funds rate 25 basis points at this meeting, as in alternative A. (9) If the Committee believed that, as in the staff forecast, a larger policy move were needed to have an adequate effect in forestalling oncoming weakness in economic activity or if it wanted to take more forceful action to address the risks facing financial markets here and abroad, it might choose to reduce the funds rate 50 basis points at this meeting (alternative A'). Those assumptions are used for the projections of money growth under alternative A. -13- the reduced attractiveness of stock mutual funds, but to a lesser degree than over the past couple months; the projected declines in stock prices are not as steep as those that already have occurred, and some of the money fund inflows at the onset of the bear market were likely only parked temporarily while in transit to alternative longer-term investments. B Debt All Alternatives Monthly Growth Rates Aug-98 Sep-98 Oct-98 Nov-98 Dec-98 Jan-99 Feb-99 Mar-99 Quarterly Averages 1998 Q1 1998 Q2 1998 Q3 1998 Q4 1999 Q1 Growth Rate From To Sep-98 Dec-98 Sep-98 Mar-99 1997 Q4 Sep-98 1997 Q4 Dec-98 1998 Q4 Mar-98 1995 Q4 1996 Q4 1996 Q4 1997 Q4 1997 Q4 1998 Q4 8.3 14.6 7.8 8.0 7.1 6.4 5.5 4.8 8.3 14.6 7.4 7.2 6.3 6.1 5,8 5.2 8.3 14.6 7.0 6.4 5.5 5.0 4.5 4.0 7.0 6.3 6.4 5.5 8.1 8.1 7.9 7.8 7.3 7.1 4.6 4.6 5.7 5.7 8.0 7.9 1998 Annual Ranges: 1.0 to 5.0 2.0 to 6.0 Note: Alternative A is consistent with the Greenbook interest rate path.</t>
   </si>
   <si>
     <t>If so, the Committee would find the unchanged stance of policy under alternative B appropriate. (11) With markets betting heavily on an easing at this FOMC meeting, holding rates unchanged as in alternative B would leave investors confused about Federal Reserve intentions and likely engender added volatility.</t>
   </si>
   <si>
+    <t>The 25 basis point easing of policy under alternative A would tend to boost most financial markets, given that the federal funds futures market evidently now has built in only about even odds of such an action at this meeting.</t>
+  </si>
+  <si>
     <t>A slight additional easing at this meeting, as in the 25 basis point reduction in the federal funds rate of alternative A, could be considered broadly in line with the policy -9- assumption underlying the staff forecast. (9) The 25 basis point easing of policy under alternative A would tend to boost most financial markets, given that the federal funds futures market evidently now has built in only about even odds of such an action at this meeting. Consequently, rates on short-term private market instruments, such as commercial paper, likely would move a little lower following implementation of alternative A. With the easing perhaps fostering additional attenuation of concerns about private credit risks, the unusual recent safe-harbor demands for Treasuries would 2 Alternative A could be implemented either through a 1/4 percentage point reduction in the discount rate to 4-1/2 percent, or through a slightly more generous provision of nonborrowed reserves, with no discount rate change, that eliminates the spread between the two rates.</t>
   </si>
   <si>
     <t>Leaving policy unchanged at this meeting, as under alternative B, would seem even more advisable if the Committee were skeptical that aggregate demand will slow to the extent forecast by the staff. (11) With many market participants likely to be disappointed by policy inaction, yields on private securities could well back up some under alternative B. M3 is forecast to outpace M2 as banks seek funding through instruments included in the broader aggregate to finance bank credit 3 The projections of money growth under alternative B assume, consistent with the Greenbook forecast, that the stance of policy is left unchanged at the November meeting and eased 25 basis points at the December meeting. Under alternative B, M2 and M3 are projected to expand over the October-to-March period at annual rates of 8 and 9-1/2 percent, respectively, leaving both aggregates by March well above the ranges established provisionally for 1999. B All Alternatives Monthly Growth Rates Jul-98 Aug-98 Sep-98 Oct-98 Nov-98 Dec-98 Jan-99 Feb-99 Mar-99 Quarterly Averages 1998 Q1 1998 Q2 1998 Q3 1998 Q4 1999 Q1 Growth Rate From To Oct-98 Dec-98 Oct-98 Mar-99 1997 1997 1998 1995 1996 1997 Oct-98 Dec-98 Mar-99 1996 Q4 1997 Q4 1998 Q4 1998 Annual Ranges: 1.0 to 5.0 2.0 to 6.0 Note: Alternative B is consistent with Greenbook forecast.</t>
   </si>
   <si>
+    <t>might rest on the view that there are substantial risks of a shortfall in global demand and of more downward pressure on prices</t>
+  </si>
+  <si>
     <t>(13) The case for easing further at some point, as in the 1/4 point reduction in the federal funds rate at this meeting of alternative A, might rest on the view that there are substantial risks of a shortfall in global demand and of more downward pressure on prices than -11- the Committee might find desirable.</t>
   </si>
   <si>
@@ -2598,6 +2616,9 @@
     <t>-10- (12) The choice of the quarter-point increase in the federal funds rate of alternative C would seem to rest on the judgment that the inflation outcome in the staff forecast is unacceptable or that there are significant risks of a more substantial pickup in inflation.</t>
   </si>
   <si>
+    <t xml:space="preserve">f the Committee remained concerned about the possibility that economic and financial weakness abroad might prove deeper and more widespread than now expected. </t>
+  </si>
+  <si>
     <t>-20- (21) The 25 basis point easing contemplated in alternative A might be seen as appropriate if the Committee remained concerned about the possibility that economic and financial weakness abroad might prove deeper and more widespread than now expected. (24) In view of the strength of recent economic activity, investors might be puzzled by implementation of alternative A, but they likely would conclude that the shift represented another small, and perhaps final, adjustment of policy to turbulence abroad designed to ensure that U.S. economic growth remained robust.</t>
   </si>
   <si>
@@ -2691,6 +2712,9 @@
     <t>(9) The FOMC instead might choose the 25 basis point increase in the federal funds rate of alternative C. Core inflation has risen and may already be above rates that Committee members find acceptable over the long run. (10) The market reaction to implementation of alternative C would likely be sharp.</t>
   </si>
   <si>
+    <t xml:space="preserve"> in order to forestall an unnecessary rise in the unemployment rate. </t>
+  </si>
+  <si>
     <t>(12) If the Committee believes that economic growth likely will remain below that of its potential at the current funds rate, along the lines of the staff forecast, but thinks that the existing level of resource use may be sustainable, then it might choose the 25 basis point easing of alternative A in order to forestall an unnecessary rise in the unemployment rate. Adoption of alternative A, therefore, would trigger a rally in bond and stock markets, though the extent would depend on the accompanying statement of the balance of risks.</t>
   </si>
   <si>
@@ -2700,6 +2724,9 @@
     <t>(10) If the Committee judges that core inflation probably will trend higher, as in the staff forecast, and finds the likely degree of economic weakness to be less of a concern, then it might want to act promptly to resist the acceleration in prices by tightening policy 25 basis points, as in alternative C.</t>
   </si>
   <si>
+    <t xml:space="preserve"> adoption of alternative A would presumably trigger a rally in bond and stock markets and a decline in the foreign exchange value of the dollar.</t>
+  </si>
+  <si>
     <t>(11) If the Committee thinks that output growth is likely to slow appreciably more than envisioned in the staff forecast, then it might choose the 25 basis point easing of alternative A. (12) With no policy move expected at this meeting, adoption of alternative A would presumably trigger a rally in bond and stock markets and a decline in the foreign exchange value of the dollar.</t>
   </si>
   <si>
@@ -2715,9 +2742,6 @@
     <t>(18) The Committee may choose the unchanged federal funds rate of alternative B if it is dissatisfied with recent rates of core inflation and wants to establish a downward trajectory for inflation, as in the price stability scenario in the second section of this bluebook.</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>ease, deg unclear</t>
   </si>
   <si>
@@ -2748,7 +2772,7 @@
     <t>Table 1: FOMC Statement Alternatives for the June Bluebook May FOMC Alternative A Alternative B Alternative C Policy Decision 1. Alternative C would boost the funds rate by 50 basis points to 1Ã‚Â½ percent. _x001A_ If so, a 50-basis-point increase in the federal funds rate, as in Alternative C, might be favored if Committee members doubt that inflation will be restrained by slack in the economy to the extent forecast by the staff, either because of skepticism about the output gap framework or concern that the economy is closer to potential than estimated by the staff, as in the _x001A_Less Room to Grow_x001A_ scenario in the Greenbook. (18) The combination of policy action and explanation proposed under Alternative C would come as a considerable shock to market participants.</t>
   </si>
   <si>
-    <t>Under Alternative A, the existing stance of policy would be maintained at this meeting. Table 1: Alternative Language for the August FOMC Announcement June FOMC Alternative A Alternative B Alternative C Policy Decision 1. _x001A_ However, if the report is again on the soft side, as in June, the Committee might wish to cite _x001A_some slowing in the pace of improvement in labor market conditions,_x001A_ as in Alternative A. (9) Although the recent pace of economic growth has been less vigorous than projected in the June Greenbook, the Committee may still judge that the economy is poised for significant expansion going forward, as in the current staff forecast. (12) If the Committee is concerned by the slow pace of progress in reducing resource slack projected in the Greenbook or is worried that the forecasted rebound in growth could fail to materialize, it may prefer the unchanged policy stance of Alternative A. _x001A_ Consistent with its motivation for selecting Alternative A, the Committee might also wish to note that policy will be adjusted as appropriate to promote _x001A_sustainable growth_x001A_ as well as price stability in the last sentence of the risk assessment section.</t>
+    <t>Under Alternative A, the existing stance of policy would be maintained at this meeting. Table 1: Alternative Language for the August FOMC Announcement June FOMC Alternative A Alternative B Alternative C Policy Decision 1.  However, if the report is again on the soft side, as in June, the Committee might wish to cite some slowing in the pace of improvement in labor market conditions, as in Alternative A. (9) Although the recent pace of economic growth has been less vigorous than projected in the June Greenbook, the Committee may still judge that the economy is poised for significant expansion going forward, as in the current staff forecast. (12) If the Committee is concerned by the slow pace of progress in reducing resource slack projected in the Greenbook or is worried that the forecasted rebound in growth could fail to materialize, it may prefer the unchanged policy stance of Alternative A.  Consistent with its motivation for selecting Alternative A, the Committee might also wish to note that policy will be adjusted as appropriate to promote sustainable growth as well as price stability in the last sentence of the risk assessment section.</t>
   </si>
   <si>
     <t>Alternative B would raise the target for the federal funds rate 25 basis points to 1_ percent. Table 1: Alternative Language for the August FOMC Announcement June FOMC Alternative A Alternative B Alternative C Policy Decision 1. If the Committee subscribes to such an outlook, it may find it appropriate to continue paring the degree of monetary policy accommodation and thus be attracted to the 25-basis-point firming at this meeting of Alternative B. (10) In announcing implementation of Alternative B, the Committee would presumably want to modify its previous statement that _x005F_x001A_output is continuing to expand at a solid pace_x005F_x001A_ to acknowledge both the softness in economic activity in the past few months and the potential effects on economic prospects of energy price developments. The inflation sentence could well be similar to that under Alternative B. (18) If the Committee favors only a modest firming in policy at this time but wishes to move away from the _x005F_x001A_measured pace_x005F_x001A_ language before long, it might wish to combine the 25-basis-point firming action and rationale of Alternative B with the conditional assessment of upside risks proposed for Alternative C.</t>
@@ -2793,7 +2817,7 @@
     <t>food and energy) (Four-quarter percent change) Strictly Confidential (FR) Class I FOMC Page 17 of 41 Table 1: Alternative Language for the January FOMC Announcement December FOMC Alternative A Alternative B Alternative C Policy Decision 1. In stark contrast, Alternative C envisions a half-point rate hike accompanied by a darker assessment of inflation risks and the removal of the _x001A_measured pace_x001A_ language. (17) If the Committee believes that a more rapid return to a neutral policy stance is needed to prevent output overshooting its potential and putting upward pressures on inflation down the road, it may choose one or all of the components included in the statement under Alternative C. 7 (18) Even if the Committee prefers a 25 basis point tightening at this meeting, it may wish to couple such a move with some of the changes in the announcement listed under Alternative C in Table 1. (19) A 50 basis point policy firming and an announcement like that indicated under Alternative C would lead to a sharp rise in short-term interest rates and a decline in bond and stock prices. Strictly Confidential (FR) Class I FOMC Page 25 of 41 attenuated, if the Committee married a quarter-point rate firming with some of the drafting language of Alternative C.</t>
   </si>
   <si>
-    <t>Under Alternative A, the funds rate also would be raised 25 basis points, but the 3 The Committee has accompanied its six prior tightenings with assessments that the risks to both of its goals were balanced, which indicates that those assessments have implicitly been conditioned on an appropriate path of policy. Class I FOMC - Restricted Controlled (FR) Page 11 of 37 Table 1: Alternative Language for the March FOMC Announcement February FOMC Alternative A Alternative B Alternative C Policy Decision 1. (14) If the Committee instead views recent higher inflation readings as largely transitory, it may wish to firm policy by a quarter point at this meeting and issue a statement like that described under Alternative A. (15) Under either Alternative A or C, the Committee may judge that the measured-pace language is no longer consistent with the likely future course of policy. Under Alternative A, the rationale paragraph would suggest that the Committee sees the stance of monetary policy as _x001A_somewhat_x001A_ accommodative and regards the recent uptick in inflation readings as transitory, with underlying inflation and inflation expectations remaining well-contained. The market reaction to adoption of Alternative A is more difficult to gauge, but the mention of cumulative firming, upbeat assessment of inflation prospects, and the characterization of the stance of policy as only _x001A_somewhat_x001A_ accommodative in the rationale paragraph should tend to put some downward pressure on yields.</t>
+    <t>Under Alternative A, the funds rate also would be raised 25 basis points, but the 3 The Committee has accompanied its six prior tightenings with assessments that the risks to both of its goals were balanced, which indicates that those assessments have implicitly been conditioned on an appropriate path of policy. Class I FOMC - Restricted Controlled (FR) Page 11 of 37 Table 1: Alternative Language for the March FOMC Announcement February FOMC Alternative A Alternative B Alternative C Policy Decision 1. (14) If the Committee instead views recent higher inflation readings as largely transitory, it may wish to firm policy by a quarter point at this meeting and issue a statement like that described under Alternative A. (15) Under either Alternative A or C, the Committee may judge that the measured-pace language is no longer consistent with the likely future course of policy. Under Alternative A, the rationale paragraph would suggest that the Committee sees the stance of monetary policy as somewhat accommodative and regards the recent uptick in inflation readings as transitory, with underlying inflation and inflation expectations remaining well-contained. The market reaction to adoption of Alternative A is more difficult to gauge, but the mention of cumulative firming, upbeat assessment of inflation prospects, and the characterization of the stance of policy as only somewhat accommodative in the rationale paragraph should tend to put some downward pressure on yields.</t>
   </si>
   <si>
     <t>Under Alternative B, the funds rate would be raised 25 basis points at this meeting. Alternative B makes the balance-of-risks assessment explicitly conditional on _x005F_x001A_appropriate policy_x005F_x001A_ and uses a more forceful verb phrase, _x005F_x001A_should be kept,_x005F_x001A_ to underscore that it may take policy action to preserve balance. However, explicitly stating that conditionality, as in Alternative B, will probably limit the usefulness of this form of the risk assessment in signaling the likely direction of future policy moves. Class I FOMC - Restricted Controlled (FR) Page 11 of 37 Table 1: Alternative Language for the March FOMC Announcement February FOMC Alternative A Alternative B Alternative C Policy Decision 1. These alternatives may contain elements of statement language that the Committee might find more appealing than the wording of Alternative B or may be helpful in informing potential changes in the policy announcement over the next few meetings. (11) If the Committee found the Greenbook forecast for output and inflation conditional on continued gradual removal of policy accommodation both plausible and acceptable, it might choose to raise the target federal funds rate _ percentage point at this meeting and issue a statement like that shown for Alternative B in Table 1. As a result, it seems likely that the market reaction to Alternative B would be fairly muted.</t>
@@ -2802,7 +2826,10 @@
     <t>Class I FOMC - Restricted Controlled (FR) Page 11 of 37 Table 1: Alternative Language for the March FOMC Announcement February FOMC Alternative A Alternative B Alternative C Policy Decision 1. Under Alternative C, the funds rate would be boosted 50 basis points, and the accompanying statement would give more emphasis to the perception of upside inflation risks. In this case, the Committee may wish to raise the target federal funds rate by 50 basis points and issue a statement like that described for Alternative C. In contrast, the language for Alternative C would suggest that output growth is proceeding at a pace that seems likely to eliminate resource slack in the near term and would note that inflation pressures have intensified, signaling a pickup in the pace of firming. (17) Market participants would be caught off guard by the 50 basis point tightening of Alternative C. The market reaction to the Class I FOMC - Restricted Controlled (FR) Page 21 of 37 language of Alternative C would be somewhat attenuated if the Committee boosted rates at this meeting by only a quarter point.</t>
   </si>
   <si>
-    <t>With some economic slack remaining, import prices rising less rapidly, and energy prices falling back somewhat as margins shrink, core PCE inflation is forecast to slow a little over the next two Class I FOMC - Restricted Controlled (FR) Page 12 of 40 Table 1: Alternative Language for the May FOMC Announcement March FOMC Alternative A Alternative B Alternative C Policy Decision 1. Alternative A would suggest that a near-term pause in the process of tightening could be in the cards. Class I FOMC - Restricted Controlled (FR) Page 18 of 40 may wish to combine a 25-basis-point firming of policy at this meeting with statement language that strongly suggests the possibility of a pause in firming at the June meeting, as in Alternative A. (15) The statement accompanying selection of Alternative A could employ virtually the same text on aggregate spending and labor market conditions suggested for Alternative B_x001A_but omitting the word _x001A_somewhat_x001A__x001A_as follows: _x001A_Recent data suggest that the solid pace of spending growth has slowed, partly in response to the earlier increases in energy prices. (16) Market participants would not likely miss the hints in the announcement of Alternative A of a higher likelihood of a pause in June.</t>
+    <t xml:space="preserve"> may wish to combine a 25-basis-point firming of policy at this meeting with statement language that strongly suggests the possibility of a pause in firming at the June meeting, as in Alternative A.</t>
+  </si>
+  <si>
+    <t>With some economic slack remaining, import prices rising less rapidly, and energy prices falling back somewhat as margins shrink, core PCE inflation is forecast to slow a little over the next two Class I FOMC - Restricted Controlled (FR) Page 12 of 40 Table 1: Alternative Language for the May FOMC Announcement March FOMC Alternative A Alternative B Alternative C Policy Decision 1. Alternative A would suggest that a near-term pause in the process of tightening could be in the cards. Class I FOMC - Restricted Controlled (FR) Page 18 of 40 may wish to combine a 25-basis-point firming of policy at this meeting with statement language that strongly suggests the possibility of a pause in firming at the June meeting, as in Alternative A. (15) The statement accompanying selection of Alternative A could employ virtually the same text on aggregate spending and labor market conditions suggested for Alternative Bbut omitting the word somewhatas follows: Recent data suggest that the solid pace of spending growth has slowed, partly in response to the earlier increases in energy prices. (16) Market participants would not likely miss the hints in the announcement of Alternative A of a higher likelihood of a pause in June.</t>
   </si>
   <si>
     <t>With some economic slack remaining, import prices rising less rapidly, and energy prices falling back somewhat as margins shrink, core PCE inflation is forecast to slow a little over the next two Class I FOMC - Restricted Controlled (FR) Page 12 of 40 Table 1: Alternative Language for the May FOMC Announcement March FOMC Alternative A Alternative B Alternative C Policy Decision 1. Apart from updating the description of recent economic conditions, the statement under Alternative B could be quite similar to that issued following the March FOMC meeting. (11) Although recent economic data have pointed to noticeably less strength in spending and output in the first half of 2005 than anticipated at the time of the March meeting, the Committee may still be inclined to tighten policy another 25-basis-point notch at this meeting, as in Alternative B. (12) The draft statement associated with Alternative B updates the wording of the March release in light of recent information on spending, employment, and inflation. _x005F_x001A_ In view of the elevated CPI figures for the past couple of months, and more generally in recognition of increased uncertainty about the interpretation of recent inflation news, the draft wording for Alternative B also suggests that the Committee omit the view expressed in March that _x005F_x001A_the rise in energy prices, however, has not notably fed through to core consumer prices. Assuming that those differing interpretations about offset each other, there is little reason to suspect that the market reaction to the adoption of Alternative B would be significant. (15) The statement accompanying selection of Alternative A could employ virtually the same text on aggregate spending and labor market conditions suggested for Alternative B_x005F_x001A_but omitting the word _x005F_x001A_somewhat_x005F_x001A__x005F_x001A_as follows: _x005F_x001A_Recent data suggest that the solid pace of spending growth has slowed, partly in response to the earlier increases in energy prices. _x005F_x001A_ Regarding inflation, the sentence offered under Alternative B could be modified under this alternative by saying, _x005F_x001A_While pressures on inflation have picked up in recent months and pricing power is more evident, longer-term inflation expectations remain well contained.</t>
@@ -2811,7 +2838,7 @@
     <t>With some economic slack remaining, import prices rising less rapidly, and energy prices falling back somewhat as margins shrink, core PCE inflation is forecast to slow a little over the next two Class I FOMC - Restricted Controlled (FR) Page 12 of 40 Table 1: Alternative Language for the May FOMC Announcement March FOMC Alternative A Alternative B Alternative C Policy Decision 1. Under Alternative C, the federal funds rate would be boosted 50 basis points, and the language would be modified substantially. (17) Should the Committee be particularly concerned that underlying inflation pressures may be intensifying, it might be attracted to the 50-basis-point increase in the federal funds rate of Alternative C. The words of Alternative C (from row 2 down) might have an appeal even if the Committee chose to firm 25 basis points at this meeting. (18) As indicated in Table 1, the Committee could consider a number of alterations to its statement in association with the selection of Alternative C to convey a heightened concern about inflation prospects. _x001A_ Class I FOMC - Restricted Controlled (FR) Page 24 of 40 (19) The selection of the 50-basis-point increase in the federal funds rate of Alternative C would come as a considerable surprise to market participants.</t>
   </si>
   <si>
-    <t>The announcement accompanying Alternative A would indicate that policy accommodation had been substantially reduced and would hint at less tightening going forward. Meanwhile, although recent inflation readings have proven reassuring, further increases in energy prices and diminishing slack in the economy may be read by Class I FOMC - Restricted Controlled (FR) 16 of 42 Table 1: Alternative Language for the June FOMC Announcement May FOMC Alternative A Alternative B Alternative C Policy Decision 1. In this case, the FOMC may be attracted to Alternative A_x001A_s combination of a 25-basis-point hike in the funds rate at this meeting and statement wording that hints that the Committee could soon pause, at least for a time, in its process of policy firming. (17) The draft statement associated with Alternative A could be explicit that _x001A_The Committee believes that the degree of monetary policy accommodation has been substantially reduced. Accordingly, a statement employing the draft wording shown in Alternative A would likely produce a noticeable downward shift in money market futures quotes, a rally in bond and equity markets, and some depreciation in the foreign exchange value of the dollar.</t>
+    <t>The announcement accompanying Alternative A would indicate that policy accommodation had been substantially reduced and would hint at less tightening going forward. Meanwhile, although recent inflation readings have proven reassuring, further increases in energy prices and diminishing slack in the economy may be read by Class I FOMC - Restricted Controlled (FR) 16 of 42 Table 1: Alternative Language for the June FOMC Announcement May FOMC Alternative A Alternative B Alternative C Policy Decision 1. In this case, the FOMC may be attracted to Alternative As combination of a 25-basis-point hike in the funds rate at this meeting and statement wording that hints that the Committee could soon pause, at least for a time, in its process of policy firming. (17) The draft statement associated with Alternative A could be explicit that The Committee believes that the degree of monetary policy accommodation has been substantially reduced. Accordingly, a statement employing the draft wording shown in Alternative A would likely produce a noticeable downward shift in money market futures quotes, a rally in bond and equity markets, and some depreciation in the foreign exchange value of the dollar.</t>
   </si>
   <si>
     <t>Apart from updating the description of the current economic situation, the announcement associated with Alternative B is little changed from that issued after the May meeting. (13) The Committee may see little reason to diverge at this point from its established precedent of measured policy firming and thus be attracted to Alternative B. Meanwhile, although recent inflation readings have proven reassuring, further increases in energy prices and diminishing slack in the economy may be read by Class I FOMC - Restricted Controlled (FR) 16 of 42 Table 1: Alternative Language for the June FOMC Announcement May FOMC Alternative A Alternative B Alternative C Policy Decision 1. (14) The announcement associated with Alternative B would update the wording of the May statement in view of incoming data on spending, output, and employment but would leave the rest of the statement unchanged.</t>
@@ -2820,7 +2847,10 @@
     <t>Under Alternative C, the Committee would raise the federal funds rate 50 basis points at this meeting, eliminate all forward-looking language, and make other significant changes to the announcement. Meanwhile, although recent inflation readings have proven reassuring, further increases in energy prices and diminishing slack in the economy may be read by Class I FOMC - Restricted Controlled (FR) 16 of 42 Table 1: Alternative Language for the June FOMC Announcement May FOMC Alternative A Alternative B Alternative C Policy Decision 1. (19) If the Committee, by contrast, has become more concerned about the potential for an upcreep in inflation in response to developments over the intermeeting period, then it may favor the 50-basis-point increase in the federal funds rate of Alternative C. (20) A number of modifications to the Committee_x001A_s statement would be required to accommodate the selection of Alternative C. (21) With nary a hint heretofore of an upshift in the pace of policy tightening, market participants would be shocked by the combination of a 50-basis-point increase in the funds rate at this meeting and the announcement suggested for Alternative C. The pairing of the language of Alternative C with a 25-basis-point move would also catch investors unawares, probably leading them to ratchet up their expectations of policy firming considerably and prompting a sell-off in fixed-income markets.</t>
   </si>
   <si>
-    <t>In contrast, the announcement accompanying Alternative A would hint at a near-term slowing in the pace of policy tightening, in part by noting that policy accommodation has been substantially reduced. Although the stance of monetary policy evidently remains accommodative, the gap between the actual real funds rate and current estimates of its equilibrium value has narrowed considerably Class I FOMC - Restricted Controlled (FR) Page 10 of 35 Table 1: Alternative Language for the August FOMC Announcement June FOMC Alternative A Alternative B Alternative C Policy Decision 1. In view of such an assessment as well as the subdued readings on core inflation in recent months, the FOMC might opt for Alternative A_x001A_s combination of a 25-basis-point hike in the funds rate at this meeting and a statement that hints that the Committee could soon slow the pace of policy firming. (14) The draft statement associated with Alternative A could indicate that _x001A_The Committee believes that the degree of monetary policy accommodation has been substantially reduced,_x001A_ while again acknowledging that the expansion remains firm and that labor market conditions continue to improve gradually. Accordingly, a statement employing the draft wording shown in Alternative A would likely produce a noticeable downward shift in interest rates implied by money market futures quotes, as investors priced in a slower pace of policy action and probably also revised down the likely extent of cumulative tightening.</t>
+    <t>Alternative As combination of a 25-basis-point hike in the funds rate at this meeting and a statement that hints that the Committee could soon slow the pace of policy firming.</t>
+  </si>
+  <si>
+    <t>In contrast, the announcement accompanying Alternative A would hint at a near-term slowing in the pace of policy tightening, in part by noting that policy accommodation has been substantially reduced. Although the stance of monetary policy evidently remains accommodative, the gap between the actual real funds rate and current estimates of its equilibrium value has narrowed considerably Class I FOMC - Restricted Controlled (FR) Page 10 of 35 Table 1: Alternative Language for the August FOMC Announcement June FOMC Alternative A Alternative B Alternative C Policy Decision 1. In view of such an assessment as well as the subdued readings on core inflation in recent months, the FOMC might opt for Alternative As combination of a 25-basis-point hike in the funds rate at this meeting and a statement that hints that the Committee could soon slow the pace of policy firming. (14) The draft statement associated with Alternative A could indicate that The Committee believes that the degree of monetary policy accommodation has been substantially reduced, while again acknowledging that the expansion remains firm and that labor market conditions continue to improve gradually. Accordingly, a statement employing the draft wording shown in Alternative A would likely produce a noticeable downward shift in interest rates implied by money market futures quotes, as investors priced in a slower pace of policy action and probably also revised down the likely extent of cumulative tightening.</t>
   </si>
   <si>
     <t>Apart from updating the description of the current economic situation, the proposed announcement associated with Alternative B is little changed from that issued after the June meeting. (10) If the Committee agrees with the staff_x005F_x001A_s assessment that a small amount of slack remains in the economy and that the current configuration of financial asset prices is likely to prove consistent with the expansion of aggregate spending coming into line with potential output growth before long, it may be attracted to the 25-basis- point firming and statement language of Alternative B. Although the stance of monetary policy evidently remains accommodative, the gap between the actual real funds rate and current estimates of its equilibrium value has narrowed considerably Class I FOMC - Restricted Controlled (FR) Page 10 of 35 Table 1: Alternative Language for the August FOMC Announcement June FOMC Alternative A Alternative B Alternative C Policy Decision 1. (11) As shown in Table 1, the statement for Alternative B updates the wording employed in June in light of incoming data on spending, output, and employment by noting that _x005F_x001A_Aggregate spending, despite high energy prices, appears to have strengthened since late winter, and labor market conditions continue to improve gradually. Thus, the market reaction to an announcement along the lines of Alternative B should be relatively modest, although rates could back up a little in response to the changes in the wording suggesting that the FOMC was focusing on the strength in spending and inflation pressures.</t>
@@ -2829,7 +2859,7 @@
     <t>The federal funds rate would be boosted 25 basis points at this meeting under Alternatives A and B, and 50 basis points under Alternative C. The proposed announcement for Alternative C emphasizes the strength of aggregate spending, suggests that pressures on business costs and inflation could be increasing, and eliminates all forward-looking language. Although the stance of monetary policy evidently remains accommodative, the gap between the actual real funds rate and current estimates of its equilibrium value has narrowed considerably Class I FOMC - Restricted Controlled (FR) Page 10 of 35 Table 1: Alternative Language for the August FOMC Announcement June FOMC Alternative A Alternative B Alternative C Policy Decision 1. (16) If the Committee has become significantly more concerned about inflation pressures of late, it may favor the 50-basis-point increase in the federal funds rate of Alternative C. (17) The Committee could consider a number of modifications to its statement in conjunction with the selection of Alternative C. (18) Market participants would no doubt be taken aback by the combination of a 50-basis-point increase in the funds rate at this meeting and the announcement suggested for Alternative C. If the FOMC were particularly concerned about inflation pressures but was not prepared to hike rates 50 basis points at this meeting, it could couple a quarter- point move with some of the changes in the statement suggested for Alternative C.</t>
   </si>
   <si>
-    <t>Under Alternative A, the Committee would leave its target for the federal funds rate unchanged at 3ÃŽÂ© percent at this meeting; the statement would emphasize hurricane-related uncertainties and suggest that this was just a pause in the tightening process. In contrast, paragraph 16 suggests wording changes to Alternative A that would be consistent with an expectation of a more prolonged pause in firming. Lastly, the box at the end of this section entitled _x001A_Opening Up the Statement_x001A_ examines fundamental changes to the risk assessment that could be made to either Alternative A or B. The Committee may view the downward revision to monetary policy expectations and the associated easing of Class I FOMC - Restricted Controlled (FR) Page 13 of 38 Table 1: Alternative Language for the September FOMC Announcement August FOMC Alternative A Alternative B Policy Decision 1. Under Alternative A, the Committee would keep the target federal funds rate unchanged at 3ÃŽÂ© percent at this meeting and use the statement to explain that it was merely deferring firming in light of the elevated uncertainties, and likely not ending the tightening cycle. The text on inflation in Alternative B could also be used in Alternative A. Such a view could be conveyed to the public by striking sentence 2 from the draft statement for Alternative A.</t>
+    <t>Under Alternative A, the Committee would leave its target for the federal funds rate unchanged at 3ÃŽÂ© percent at this meeting; the statement would emphasize hurricane-related uncertainties and suggest that this was just a pause in the tightening process. In contrast, paragraph 16 suggests wording changes to Alternative A that would be consistent with an expectation of a more prolonged pause in firming. Lastly, the box at the end of this section entitled Opening Up the Statement examines fundamental changes to the risk assessment that could be made to either Alternative A or B. The Committee may view the downward revision to monetary policy expectations and the associated easing of Class I FOMC - Restricted Controlled (FR) Page 13 of 38 Table 1: Alternative Language for the September FOMC Announcement August FOMC Alternative A Alternative B Policy Decision 1. Under Alternative A, the Committee would keep the target federal funds rate unchanged at 3ÃŽÂ© percent at this meeting and use the statement to explain that it was merely deferring firming in light of the elevated uncertainties, and likely not ending the tightening cycle. The text on inflation in Alternative B could also be used in Alternative A. Such a view could be conveyed to the public by striking sentence 2 from the draft statement for Alternative A.</t>
   </si>
   <si>
     <t>Under Alternative B, the Committee would boost the target 25 basis points to 3_ percent; the statement would note that the longer-term macroeconomic effects of the hurricane are likely to be limited. Paragraph 13 considers changes to the statement language (relative to Alternative B) that could express more concern about inflation. (10) If the Committee remains particularly concerned about heightened inflation pressures and sees little chance that Hurricane Katrina will have lasting and sizable adverse effects on aggregate spending and production, it may wish to tighten policy 25 basis points at this meeting, as under Alternative B. The Committee may view the downward revision to monetary policy expectations and the associated easing of Class I FOMC - Restricted Controlled (FR) Page 13 of 38 Table 1: Alternative Language for the September FOMC Announcement August FOMC Alternative A Alternative B Policy Decision 1. (11) As shown in Table 1, the proposed announcement associated with Alternative B would indicate that _x005F_x001A_Output appeared poised to continue growing at a good pace before the tragic toll of Hurricane Katrina. If the Committee saw this inflation outcome as unacceptable or believed that such an expectation was likely to prove optimistic, then it might view the words of Alternative B as too timid about the prospects for additional policy tightening. The likelihood of more tightening than currently built into financial market prices could be conveyed to the public by shortening the wording for Alternative B that appears in Table 1. Class I FOMC - Restricted Controlled (FR) Page 21 of 38 accepting the economic outlook discussed under Alternative B, members may harbor the reservation that there is a small probability that the disruption to economic activity in the Gulf region and sapping of consumer and business confidence nationwide could have serious consequences for the broader economy. As in Alternative B, the Committee could note the adverse near-term effects of the hurricane on spending, production, and employment, but not include the sentence suggesting that the effects will be temporary. The text on inflation in Alternative B could also be used in Alternative A.</t>
@@ -2848,6 +2878,9 @@
   </si>
   <si>
     <t>Given the absence of major surprises in the economic and financial environment during the intermeeting Class I FOMC - Restricted Controlled (FR) Page 12 of 42 Class I FOMC _x001A_ Restricted Controlled FR Table 1: Alternative Language for the December FOMC Announcement November FOMC Alternative B Alternative C Policy Decision 1. By contrast, Alternative C retains much of the form as well as important elements of the content of the November FOMC statement, including the characterization of policy as accommodative and the _x001A_measured pace_x001A_ language. However, the rationale section of Alternative C would convey greater concerns about inflation than the comparable portion of Alternative B. Alternative C (15) Should the Committee be particularly concerned about the inflation outlook and still see the stance of policy as accommodative, it may prefer Alternative C. (17) Release of the statement for Alternative C would lead market participants to boost noticeably their expectations for policy tightening.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While the Greenbook projections for economic growth and inflation have been revised up for this year, the current level of the output gap is slightly wider owing to a greater-than- Class I FOMC - Restricted Controlled (FR) </t>
   </si>
   <si>
     <t>The target funds rate would be raised 25 basis points under Alternatives B and C but left unchanged under Alternative A. While the Greenbook projections for economic growth and inflation have been revised up for this year, the current level of the output gap is slightly wider owing to a greater-than- Class I FOMC - Restricted Controlled (FR) Page 17 of 42 Table 1: Alternative Language for the January FOMC Announcement December FOMC Alternative A Alternative B Alternative C Policy Decision 1. (19) If members see sizable odds that the target funds rate has already been raised sufficiently to check inflationary pressures, the Committee would presumably choose to forego a policy move at this meeting, as in Alternative A. (20) The proposed wording of inflation concerns for Alternative A, in row 3 of Table 1, is basically a reordering of the sentences employed in the last announcement.</t>
@@ -3951,8 +3984,8 @@
   <dimension ref="A1:AA376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A262" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I271" sqref="I271"/>
+      <pane ySplit="1" topLeftCell="A268" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA1" sqref="AA1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3963,6 +3996,8 @@
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="44" customWidth="1"/>
+    <col min="26" max="26" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -15642,20 +15677,26 @@
       <c r="G287" t="s">
         <v>567</v>
       </c>
+      <c r="H287">
+        <v>-0.25</v>
+      </c>
+      <c r="I287" t="s">
+        <v>836</v>
+      </c>
       <c r="J287" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="K287" t="s">
         <v>569</v>
       </c>
       <c r="N287" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="O287" t="s">
         <v>574</v>
       </c>
       <c r="R287" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="V287" t="s">
         <v>30</v>
@@ -15686,20 +15727,26 @@
       <c r="G288" t="s">
         <v>567</v>
       </c>
+      <c r="H288">
+        <v>-0.25</v>
+      </c>
+      <c r="I288" t="s">
+        <v>840</v>
+      </c>
       <c r="J288" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="K288" t="s">
         <v>569</v>
       </c>
       <c r="N288" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="O288" t="s">
         <v>571</v>
       </c>
       <c r="R288" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="V288" t="s">
         <v>30</v>
@@ -15730,6 +15777,9 @@
       <c r="G289" t="s">
         <v>583</v>
       </c>
+      <c r="H289" t="s">
+        <v>844</v>
+      </c>
       <c r="J289" t="s">
         <v>27</v>
       </c>
@@ -15737,13 +15787,13 @@
         <v>569</v>
       </c>
       <c r="N289" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="O289" t="s">
         <v>571</v>
       </c>
       <c r="R289" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="V289" t="s">
         <v>30</v>
@@ -15774,6 +15824,9 @@
       <c r="G290" t="s">
         <v>583</v>
       </c>
+      <c r="H290" t="s">
+        <v>844</v>
+      </c>
       <c r="J290" t="s">
         <v>27</v>
       </c>
@@ -15781,13 +15834,13 @@
         <v>569</v>
       </c>
       <c r="N290" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="O290" t="s">
         <v>571</v>
       </c>
       <c r="R290" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="V290" t="s">
         <v>30</v>
@@ -15818,20 +15871,23 @@
       <c r="G291" t="s">
         <v>567</v>
       </c>
+      <c r="H291">
+        <v>-0.25</v>
+      </c>
       <c r="J291" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="K291" t="s">
         <v>569</v>
       </c>
       <c r="N291" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="O291" t="s">
         <v>571</v>
       </c>
       <c r="R291" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="V291" t="s">
         <v>30</v>
@@ -15862,14 +15918,20 @@
       <c r="G292" t="s">
         <v>567</v>
       </c>
+      <c r="H292">
+        <v>-0.25</v>
+      </c>
+      <c r="I292" t="s">
+        <v>852</v>
+      </c>
       <c r="J292" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="K292" t="s">
         <v>569</v>
       </c>
       <c r="N292" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="O292" t="s">
         <v>583</v>
@@ -15906,14 +15968,20 @@
       <c r="G293" t="s">
         <v>567</v>
       </c>
+      <c r="H293">
+        <v>-0.25</v>
+      </c>
+      <c r="I293" t="s">
+        <v>855</v>
+      </c>
       <c r="J293" t="s">
-        <v>851</v>
+        <v>856</v>
       </c>
       <c r="K293" t="s">
         <v>569</v>
       </c>
       <c r="N293" t="s">
-        <v>852</v>
+        <v>857</v>
       </c>
       <c r="O293" t="s">
         <v>583</v>
@@ -15950,20 +16018,26 @@
       <c r="G294" t="s">
         <v>567</v>
       </c>
+      <c r="H294">
+        <v>-0.25</v>
+      </c>
+      <c r="I294" t="s">
+        <v>858</v>
+      </c>
       <c r="J294" t="s">
-        <v>853</v>
+        <v>859</v>
       </c>
       <c r="K294" t="s">
         <v>569</v>
       </c>
       <c r="N294" t="s">
-        <v>854</v>
+        <v>860</v>
       </c>
       <c r="O294" t="s">
         <v>571</v>
       </c>
       <c r="R294" t="s">
-        <v>855</v>
+        <v>861</v>
       </c>
       <c r="V294" t="s">
         <v>30</v>
@@ -15994,20 +16068,26 @@
       <c r="G295" t="s">
         <v>567</v>
       </c>
+      <c r="H295">
+        <v>-0.25</v>
+      </c>
+      <c r="I295" t="s">
+        <v>862</v>
+      </c>
       <c r="J295" t="s">
-        <v>856</v>
+        <v>863</v>
       </c>
       <c r="K295" t="s">
         <v>569</v>
       </c>
       <c r="N295" t="s">
-        <v>857</v>
+        <v>864</v>
       </c>
       <c r="O295" t="s">
         <v>571</v>
       </c>
       <c r="R295" t="s">
-        <v>858</v>
+        <v>865</v>
       </c>
       <c r="V295" t="s">
         <v>30</v>
@@ -16038,6 +16118,9 @@
       <c r="G296" t="s">
         <v>583</v>
       </c>
+      <c r="H296" t="s">
+        <v>844</v>
+      </c>
       <c r="J296" t="s">
         <v>27</v>
       </c>
@@ -16045,13 +16128,13 @@
         <v>569</v>
       </c>
       <c r="N296" t="s">
-        <v>859</v>
+        <v>866</v>
       </c>
       <c r="O296" t="s">
         <v>571</v>
       </c>
       <c r="R296" t="s">
-        <v>860</v>
+        <v>867</v>
       </c>
       <c r="V296" t="s">
         <v>30</v>
@@ -16082,6 +16165,9 @@
       <c r="G297" t="s">
         <v>583</v>
       </c>
+      <c r="H297" t="s">
+        <v>844</v>
+      </c>
       <c r="J297" t="s">
         <v>27</v>
       </c>
@@ -16089,13 +16175,13 @@
         <v>569</v>
       </c>
       <c r="N297" t="s">
-        <v>861</v>
+        <v>868</v>
       </c>
       <c r="O297" t="s">
         <v>571</v>
       </c>
       <c r="R297" t="s">
-        <v>862</v>
+        <v>869</v>
       </c>
       <c r="V297" t="s">
         <v>30</v>
@@ -16126,6 +16212,9 @@
       <c r="G298" t="s">
         <v>583</v>
       </c>
+      <c r="H298" t="s">
+        <v>844</v>
+      </c>
       <c r="J298" t="s">
         <v>27</v>
       </c>
@@ -16133,13 +16222,13 @@
         <v>569</v>
       </c>
       <c r="N298" t="s">
-        <v>863</v>
+        <v>870</v>
       </c>
       <c r="O298" t="s">
         <v>571</v>
       </c>
       <c r="R298" t="s">
-        <v>864</v>
+        <v>871</v>
       </c>
       <c r="V298" t="s">
         <v>30</v>
@@ -16170,6 +16259,9 @@
       <c r="G299" t="s">
         <v>583</v>
       </c>
+      <c r="H299" t="s">
+        <v>844</v>
+      </c>
       <c r="J299" t="s">
         <v>27</v>
       </c>
@@ -16177,13 +16269,13 @@
         <v>569</v>
       </c>
       <c r="N299" t="s">
-        <v>865</v>
+        <v>872</v>
       </c>
       <c r="O299" t="s">
         <v>571</v>
       </c>
       <c r="R299" t="s">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="V299" t="s">
         <v>30</v>
@@ -16214,6 +16306,9 @@
       <c r="G300" t="s">
         <v>583</v>
       </c>
+      <c r="H300" t="s">
+        <v>844</v>
+      </c>
       <c r="J300" t="s">
         <v>27</v>
       </c>
@@ -16221,13 +16316,13 @@
         <v>569</v>
       </c>
       <c r="N300" t="s">
-        <v>867</v>
+        <v>874</v>
       </c>
       <c r="O300" t="s">
         <v>571</v>
       </c>
       <c r="R300" t="s">
-        <v>868</v>
+        <v>875</v>
       </c>
       <c r="V300" t="s">
         <v>30</v>
@@ -16258,6 +16353,9 @@
       <c r="G301" t="s">
         <v>583</v>
       </c>
+      <c r="H301" t="s">
+        <v>844</v>
+      </c>
       <c r="J301" t="s">
         <v>27</v>
       </c>
@@ -16265,13 +16363,13 @@
         <v>569</v>
       </c>
       <c r="N301" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="O301" t="s">
         <v>571</v>
       </c>
       <c r="R301" t="s">
-        <v>870</v>
+        <v>877</v>
       </c>
       <c r="V301" t="s">
         <v>30</v>
@@ -16302,6 +16400,9 @@
       <c r="G302" t="s">
         <v>583</v>
       </c>
+      <c r="H302" t="s">
+        <v>844</v>
+      </c>
       <c r="J302" t="s">
         <v>27</v>
       </c>
@@ -16309,13 +16410,13 @@
         <v>569</v>
       </c>
       <c r="N302" t="s">
-        <v>871</v>
+        <v>878</v>
       </c>
       <c r="O302" t="s">
         <v>571</v>
       </c>
       <c r="R302" t="s">
-        <v>872</v>
+        <v>879</v>
       </c>
       <c r="V302" t="s">
         <v>30</v>
@@ -16346,6 +16447,9 @@
       <c r="G303" t="s">
         <v>583</v>
       </c>
+      <c r="H303" t="s">
+        <v>844</v>
+      </c>
       <c r="J303" t="s">
         <v>27</v>
       </c>
@@ -16353,16 +16457,16 @@
         <v>569</v>
       </c>
       <c r="N303" t="s">
-        <v>873</v>
+        <v>880</v>
       </c>
       <c r="O303" t="s">
         <v>571</v>
       </c>
       <c r="R303" t="s">
-        <v>874</v>
+        <v>881</v>
       </c>
       <c r="V303" t="s">
-        <v>875</v>
+        <v>882</v>
       </c>
       <c r="Z303" t="s">
         <v>31</v>
@@ -16390,6 +16494,9 @@
       <c r="G304" t="s">
         <v>583</v>
       </c>
+      <c r="H304" t="s">
+        <v>844</v>
+      </c>
       <c r="J304" t="s">
         <v>27</v>
       </c>
@@ -16397,16 +16504,16 @@
         <v>569</v>
       </c>
       <c r="N304" t="s">
-        <v>876</v>
+        <v>883</v>
       </c>
       <c r="O304" t="s">
         <v>571</v>
       </c>
       <c r="R304" t="s">
-        <v>877</v>
+        <v>884</v>
       </c>
       <c r="V304" t="s">
-        <v>878</v>
+        <v>885</v>
       </c>
       <c r="Z304" t="s">
         <v>31</v>
@@ -16434,6 +16541,9 @@
       <c r="G305" t="s">
         <v>583</v>
       </c>
+      <c r="H305" t="s">
+        <v>844</v>
+      </c>
       <c r="J305" t="s">
         <v>27</v>
       </c>
@@ -16447,10 +16557,10 @@
         <v>571</v>
       </c>
       <c r="R305" t="s">
-        <v>879</v>
+        <v>886</v>
       </c>
       <c r="V305" t="s">
-        <v>880</v>
+        <v>887</v>
       </c>
       <c r="Z305" t="s">
         <v>31</v>
@@ -16478,6 +16588,9 @@
       <c r="G306" t="s">
         <v>583</v>
       </c>
+      <c r="H306" t="s">
+        <v>844</v>
+      </c>
       <c r="J306" t="s">
         <v>27</v>
       </c>
@@ -16485,13 +16598,13 @@
         <v>569</v>
       </c>
       <c r="N306" t="s">
-        <v>881</v>
+        <v>888</v>
       </c>
       <c r="O306" t="s">
         <v>571</v>
       </c>
       <c r="R306" t="s">
-        <v>882</v>
+        <v>889</v>
       </c>
       <c r="V306" t="s">
         <v>30</v>
@@ -16522,6 +16635,9 @@
       <c r="G307" t="s">
         <v>583</v>
       </c>
+      <c r="H307" t="s">
+        <v>844</v>
+      </c>
       <c r="J307" t="s">
         <v>27</v>
       </c>
@@ -16529,13 +16645,13 @@
         <v>569</v>
       </c>
       <c r="N307" t="s">
-        <v>883</v>
+        <v>890</v>
       </c>
       <c r="O307" t="s">
         <v>571</v>
       </c>
       <c r="R307" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="V307" t="s">
         <v>30</v>
@@ -16566,6 +16682,9 @@
       <c r="G308" t="s">
         <v>583</v>
       </c>
+      <c r="H308" t="s">
+        <v>844</v>
+      </c>
       <c r="J308" t="s">
         <v>27</v>
       </c>
@@ -16573,13 +16692,13 @@
         <v>569</v>
       </c>
       <c r="N308" t="s">
-        <v>885</v>
+        <v>892</v>
       </c>
       <c r="O308" t="s">
         <v>571</v>
       </c>
       <c r="R308" t="s">
-        <v>886</v>
+        <v>893</v>
       </c>
       <c r="V308" t="s">
         <v>30</v>
@@ -16610,20 +16729,26 @@
       <c r="G309" t="s">
         <v>567</v>
       </c>
+      <c r="H309">
+        <v>-0.25</v>
+      </c>
+      <c r="I309" t="s">
+        <v>894</v>
+      </c>
       <c r="J309" t="s">
-        <v>887</v>
+        <v>895</v>
       </c>
       <c r="K309" t="s">
         <v>569</v>
       </c>
       <c r="N309" t="s">
-        <v>888</v>
+        <v>896</v>
       </c>
       <c r="O309" t="s">
         <v>571</v>
       </c>
       <c r="R309" t="s">
-        <v>889</v>
+        <v>897</v>
       </c>
       <c r="V309" t="s">
         <v>30</v>
@@ -16654,20 +16779,26 @@
       <c r="G310" t="s">
         <v>567</v>
       </c>
+      <c r="H310">
+        <v>-0.25</v>
+      </c>
+      <c r="I310" t="s">
+        <v>898</v>
+      </c>
       <c r="J310" t="s">
-        <v>890</v>
+        <v>899</v>
       </c>
       <c r="K310" t="s">
         <v>569</v>
       </c>
       <c r="N310" t="s">
-        <v>891</v>
+        <v>900</v>
       </c>
       <c r="O310" t="s">
         <v>571</v>
       </c>
       <c r="R310" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="V310" t="s">
         <v>30</v>
@@ -16699,19 +16830,19 @@
         <v>567</v>
       </c>
       <c r="H311">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="J311" t="s">
-        <v>893</v>
+        <v>902</v>
       </c>
       <c r="K311" t="s">
         <v>569</v>
       </c>
       <c r="L311">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="N311" t="s">
-        <v>894</v>
+        <v>903</v>
       </c>
       <c r="O311" t="s">
         <v>583</v>
@@ -16752,7 +16883,7 @@
         <v>583</v>
       </c>
       <c r="H312">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="J312" t="s">
         <v>27</v>
@@ -16761,7 +16892,7 @@
         <v>583</v>
       </c>
       <c r="L312">
-        <v>-75</v>
+        <v>-0.75</v>
       </c>
       <c r="N312" t="s">
         <v>28</v>
@@ -16770,7 +16901,7 @@
         <v>583</v>
       </c>
       <c r="P312">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="R312" t="s">
         <v>29</v>
@@ -16805,7 +16936,7 @@
         <v>583</v>
       </c>
       <c r="H313">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="J313" t="s">
         <v>27</v>
@@ -16814,7 +16945,7 @@
         <v>583</v>
       </c>
       <c r="L313">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N313" t="s">
         <v>28</v>
@@ -16823,7 +16954,7 @@
         <v>583</v>
       </c>
       <c r="P313">
-        <v>-75</v>
+        <v>-0.75</v>
       </c>
       <c r="R313" t="s">
         <v>29</v>
@@ -16867,7 +16998,7 @@
         <v>583</v>
       </c>
       <c r="L314">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N314" t="s">
         <v>28</v>
@@ -16876,7 +17007,7 @@
         <v>583</v>
       </c>
       <c r="P314">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="R314" t="s">
         <v>29</v>
@@ -16920,7 +17051,7 @@
         <v>583</v>
       </c>
       <c r="L315">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N315" t="s">
         <v>28</v>
@@ -16929,7 +17060,7 @@
         <v>583</v>
       </c>
       <c r="P315">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="R315" t="s">
         <v>29</v>
@@ -16964,7 +17095,7 @@
         <v>583</v>
       </c>
       <c r="H316">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="J316" t="s">
         <v>27</v>
@@ -16973,7 +17104,7 @@
         <v>583</v>
       </c>
       <c r="L316">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N316" t="s">
         <v>28</v>
@@ -16982,7 +17113,7 @@
         <v>583</v>
       </c>
       <c r="P316" t="s">
-        <v>895</v>
+        <v>844</v>
       </c>
       <c r="R316" t="s">
         <v>29</v>
@@ -17026,7 +17157,7 @@
         <v>583</v>
       </c>
       <c r="L317">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N317" t="s">
         <v>28</v>
@@ -17035,7 +17166,7 @@
         <v>583</v>
       </c>
       <c r="P317">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="R317" t="s">
         <v>29</v>
@@ -17079,7 +17210,7 @@
         <v>583</v>
       </c>
       <c r="L318">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N318" t="s">
         <v>28</v>
@@ -17088,7 +17219,7 @@
         <v>583</v>
       </c>
       <c r="P318">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="R318" t="s">
         <v>29</v>
@@ -17132,7 +17263,7 @@
         <v>583</v>
       </c>
       <c r="L319">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N319" t="s">
         <v>28</v>
@@ -17141,7 +17272,7 @@
         <v>583</v>
       </c>
       <c r="P319" t="s">
-        <v>895</v>
+        <v>844</v>
       </c>
       <c r="R319" t="s">
         <v>29</v>
@@ -17176,7 +17307,7 @@
         <v>583</v>
       </c>
       <c r="H320">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="J320" t="s">
         <v>27</v>
@@ -17194,7 +17325,7 @@
         <v>583</v>
       </c>
       <c r="P320">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="R320" t="s">
         <v>29</v>
@@ -17238,7 +17369,7 @@
         <v>583</v>
       </c>
       <c r="L321" t="s">
-        <v>896</v>
+        <v>904</v>
       </c>
       <c r="N321" t="s">
         <v>28</v>
@@ -17247,7 +17378,7 @@
         <v>583</v>
       </c>
       <c r="P321">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="R321" t="s">
         <v>29</v>
@@ -17291,7 +17422,7 @@
         <v>583</v>
       </c>
       <c r="L322">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N322" t="s">
         <v>28</v>
@@ -17300,7 +17431,7 @@
         <v>583</v>
       </c>
       <c r="P322">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="R322" t="s">
         <v>29</v>
@@ -17344,7 +17475,7 @@
         <v>583</v>
       </c>
       <c r="L323">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N323" t="s">
         <v>28</v>
@@ -17353,7 +17484,7 @@
         <v>583</v>
       </c>
       <c r="P323" t="s">
-        <v>895</v>
+        <v>844</v>
       </c>
       <c r="R323" t="s">
         <v>29</v>
@@ -17397,7 +17528,7 @@
         <v>583</v>
       </c>
       <c r="L324">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N324" t="s">
         <v>28</v>
@@ -17406,7 +17537,7 @@
         <v>583</v>
       </c>
       <c r="P324">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="R324" t="s">
         <v>29</v>
@@ -17450,7 +17581,7 @@
         <v>583</v>
       </c>
       <c r="L325">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N325" t="s">
         <v>28</v>
@@ -17459,7 +17590,7 @@
         <v>583</v>
       </c>
       <c r="P325">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="R325" t="s">
         <v>29</v>
@@ -17503,7 +17634,7 @@
         <v>583</v>
       </c>
       <c r="L326">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N326" t="s">
         <v>28</v>
@@ -17512,7 +17643,7 @@
         <v>583</v>
       </c>
       <c r="P326" t="s">
-        <v>895</v>
+        <v>844</v>
       </c>
       <c r="R326" t="s">
         <v>29</v>
@@ -17556,7 +17687,7 @@
         <v>583</v>
       </c>
       <c r="L327">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N327" t="s">
         <v>28</v>
@@ -17565,7 +17696,7 @@
         <v>583</v>
       </c>
       <c r="P327" t="s">
-        <v>895</v>
+        <v>844</v>
       </c>
       <c r="R327" t="s">
         <v>29</v>
@@ -17609,7 +17740,7 @@
         <v>583</v>
       </c>
       <c r="L328">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N328" t="s">
         <v>28</v>
@@ -17618,7 +17749,7 @@
         <v>583</v>
       </c>
       <c r="P328">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="R328" t="s">
         <v>29</v>
@@ -17662,7 +17793,7 @@
         <v>583</v>
       </c>
       <c r="L329">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N329" t="s">
         <v>28</v>
@@ -17671,7 +17802,7 @@
         <v>583</v>
       </c>
       <c r="P329">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="R329" t="s">
         <v>29</v>
@@ -17706,7 +17837,7 @@
         <v>583</v>
       </c>
       <c r="H330">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="J330" t="s">
         <v>27</v>
@@ -17715,7 +17846,7 @@
         <v>583</v>
       </c>
       <c r="L330">
-        <v>-50</v>
+        <v>-0.5</v>
       </c>
       <c r="N330" t="s">
         <v>28</v>
@@ -17768,7 +17899,7 @@
         <v>583</v>
       </c>
       <c r="L331">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N331" t="s">
         <v>28</v>
@@ -17777,7 +17908,7 @@
         <v>583</v>
       </c>
       <c r="P331" t="s">
-        <v>895</v>
+        <v>844</v>
       </c>
       <c r="R331" t="s">
         <v>29</v>
@@ -17821,7 +17952,7 @@
         <v>583</v>
       </c>
       <c r="L332">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N332" t="s">
         <v>28</v>
@@ -17830,7 +17961,7 @@
         <v>583</v>
       </c>
       <c r="P332" t="s">
-        <v>895</v>
+        <v>844</v>
       </c>
       <c r="R332" t="s">
         <v>29</v>
@@ -17874,7 +18005,7 @@
         <v>583</v>
       </c>
       <c r="L333">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N333" t="s">
         <v>28</v>
@@ -17883,7 +18014,7 @@
         <v>583</v>
       </c>
       <c r="P333" t="s">
-        <v>895</v>
+        <v>844</v>
       </c>
       <c r="R333" t="s">
         <v>29</v>
@@ -17927,7 +18058,7 @@
         <v>583</v>
       </c>
       <c r="L334">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N334" t="s">
         <v>28</v>
@@ -17936,7 +18067,7 @@
         <v>583</v>
       </c>
       <c r="P334" t="s">
-        <v>895</v>
+        <v>844</v>
       </c>
       <c r="R334" t="s">
         <v>29</v>
@@ -17980,7 +18111,7 @@
         <v>583</v>
       </c>
       <c r="L335">
-        <v>-25</v>
+        <v>-0.25</v>
       </c>
       <c r="N335" t="s">
         <v>28</v>
@@ -17989,7 +18120,7 @@
         <v>583</v>
       </c>
       <c r="P335">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="R335" t="s">
         <v>29</v>
@@ -18023,20 +18154,23 @@
       <c r="G336" t="s">
         <v>574</v>
       </c>
+      <c r="H336" t="s">
+        <v>574</v>
+      </c>
       <c r="J336" t="s">
-        <v>897</v>
+        <v>905</v>
       </c>
       <c r="K336" t="s">
         <v>574</v>
       </c>
       <c r="N336" t="s">
-        <v>898</v>
+        <v>906</v>
       </c>
       <c r="O336" t="s">
         <v>574</v>
       </c>
       <c r="R336" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="V336" t="s">
         <v>30</v>
@@ -18067,20 +18201,23 @@
       <c r="G337" t="s">
         <v>574</v>
       </c>
+      <c r="H337" t="s">
+        <v>574</v>
+      </c>
       <c r="J337" t="s">
-        <v>900</v>
+        <v>908</v>
       </c>
       <c r="K337" t="s">
         <v>571</v>
       </c>
       <c r="N337" t="s">
-        <v>901</v>
+        <v>909</v>
       </c>
       <c r="O337" t="s">
         <v>571</v>
       </c>
       <c r="R337" t="s">
-        <v>902</v>
+        <v>910</v>
       </c>
       <c r="V337" t="s">
         <v>30</v>
@@ -18111,20 +18248,23 @@
       <c r="G338" t="s">
         <v>569</v>
       </c>
+      <c r="H338">
+        <v>0</v>
+      </c>
       <c r="J338" t="s">
-        <v>903</v>
+        <v>911</v>
       </c>
       <c r="K338" t="s">
         <v>571</v>
       </c>
       <c r="N338" t="s">
-        <v>904</v>
+        <v>912</v>
       </c>
       <c r="O338" t="s">
         <v>571</v>
       </c>
       <c r="R338" t="s">
-        <v>905</v>
+        <v>913</v>
       </c>
       <c r="V338" t="s">
         <v>30</v>
@@ -18155,20 +18295,23 @@
       <c r="G339" t="s">
         <v>569</v>
       </c>
+      <c r="H339">
+        <v>0</v>
+      </c>
       <c r="J339" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="K339" t="s">
         <v>571</v>
       </c>
       <c r="N339" t="s">
-        <v>907</v>
+        <v>915</v>
       </c>
       <c r="O339" t="s">
         <v>571</v>
       </c>
       <c r="R339" t="s">
-        <v>908</v>
+        <v>916</v>
       </c>
       <c r="V339" t="s">
         <v>30</v>
@@ -18199,20 +18342,23 @@
       <c r="G340" t="s">
         <v>569</v>
       </c>
+      <c r="H340">
+        <v>0</v>
+      </c>
       <c r="J340" t="s">
-        <v>909</v>
+        <v>917</v>
       </c>
       <c r="K340" t="s">
         <v>571</v>
       </c>
       <c r="N340" t="s">
-        <v>910</v>
+        <v>918</v>
       </c>
       <c r="O340" t="s">
         <v>571</v>
       </c>
       <c r="R340" t="s">
-        <v>911</v>
+        <v>919</v>
       </c>
       <c r="V340" t="s">
         <v>30</v>
@@ -18243,20 +18389,23 @@
       <c r="G341" t="s">
         <v>569</v>
       </c>
+      <c r="H341">
+        <v>0</v>
+      </c>
       <c r="J341" t="s">
-        <v>912</v>
+        <v>920</v>
       </c>
       <c r="K341" t="s">
         <v>571</v>
       </c>
       <c r="N341" t="s">
-        <v>913</v>
+        <v>921</v>
       </c>
       <c r="O341" t="s">
         <v>571</v>
       </c>
       <c r="R341" t="s">
-        <v>914</v>
+        <v>922</v>
       </c>
       <c r="V341" t="s">
         <v>30</v>
@@ -18287,20 +18436,23 @@
       <c r="G342" t="s">
         <v>569</v>
       </c>
+      <c r="H342">
+        <v>0</v>
+      </c>
       <c r="J342" t="s">
-        <v>915</v>
+        <v>923</v>
       </c>
       <c r="K342" t="s">
         <v>571</v>
       </c>
       <c r="N342" t="s">
-        <v>916</v>
+        <v>924</v>
       </c>
       <c r="O342" t="s">
         <v>571</v>
       </c>
       <c r="R342" t="s">
-        <v>917</v>
+        <v>925</v>
       </c>
       <c r="V342" t="s">
         <v>30</v>
@@ -18331,20 +18483,23 @@
       <c r="G343" t="s">
         <v>569</v>
       </c>
+      <c r="H343">
+        <v>0</v>
+      </c>
       <c r="J343" t="s">
-        <v>918</v>
+        <v>926</v>
       </c>
       <c r="K343" t="s">
         <v>571</v>
       </c>
       <c r="N343" t="s">
-        <v>919</v>
+        <v>927</v>
       </c>
       <c r="O343" t="s">
         <v>571</v>
       </c>
       <c r="R343" t="s">
-        <v>920</v>
+        <v>928</v>
       </c>
       <c r="V343" t="s">
         <v>30</v>
@@ -18375,20 +18530,23 @@
       <c r="G344" t="s">
         <v>571</v>
       </c>
+      <c r="H344">
+        <v>0.25</v>
+      </c>
       <c r="J344" t="s">
-        <v>921</v>
+        <v>929</v>
       </c>
       <c r="K344" t="s">
         <v>571</v>
       </c>
       <c r="N344" t="s">
-        <v>922</v>
+        <v>930</v>
       </c>
       <c r="O344" t="s">
         <v>571</v>
       </c>
       <c r="R344" t="s">
-        <v>923</v>
+        <v>931</v>
       </c>
       <c r="V344" t="s">
         <v>30</v>
@@ -18419,20 +18577,26 @@
       <c r="G345" t="s">
         <v>571</v>
       </c>
+      <c r="H345">
+        <v>0.25</v>
+      </c>
+      <c r="I345" t="s">
+        <v>932</v>
+      </c>
       <c r="J345" t="s">
-        <v>924</v>
+        <v>933</v>
       </c>
       <c r="K345" t="s">
         <v>571</v>
       </c>
       <c r="N345" t="s">
-        <v>925</v>
+        <v>934</v>
       </c>
       <c r="O345" t="s">
         <v>571</v>
       </c>
       <c r="R345" t="s">
-        <v>926</v>
+        <v>935</v>
       </c>
       <c r="V345" t="s">
         <v>30</v>
@@ -18463,20 +18627,26 @@
       <c r="G346" t="s">
         <v>571</v>
       </c>
+      <c r="H346">
+        <v>0.25</v>
+      </c>
+      <c r="I346" t="s">
+        <v>932</v>
+      </c>
       <c r="J346" t="s">
-        <v>927</v>
+        <v>936</v>
       </c>
       <c r="K346" t="s">
         <v>571</v>
       </c>
       <c r="N346" t="s">
-        <v>928</v>
+        <v>937</v>
       </c>
       <c r="O346" t="s">
         <v>571</v>
       </c>
       <c r="R346" t="s">
-        <v>929</v>
+        <v>938</v>
       </c>
       <c r="V346" t="s">
         <v>30</v>
@@ -18507,20 +18677,26 @@
       <c r="G347" t="s">
         <v>571</v>
       </c>
+      <c r="H347">
+        <v>0.25</v>
+      </c>
+      <c r="I347" t="s">
+        <v>939</v>
+      </c>
       <c r="J347" t="s">
-        <v>930</v>
+        <v>940</v>
       </c>
       <c r="K347" t="s">
         <v>571</v>
       </c>
       <c r="N347" t="s">
-        <v>931</v>
+        <v>941</v>
       </c>
       <c r="O347" t="s">
         <v>571</v>
       </c>
       <c r="R347" t="s">
-        <v>932</v>
+        <v>942</v>
       </c>
       <c r="V347" t="s">
         <v>30</v>
@@ -18551,14 +18727,17 @@
       <c r="G348" t="s">
         <v>569</v>
       </c>
+      <c r="H348">
+        <v>0</v>
+      </c>
       <c r="J348" t="s">
-        <v>933</v>
+        <v>943</v>
       </c>
       <c r="K348" t="s">
         <v>571</v>
       </c>
       <c r="N348" t="s">
-        <v>934</v>
+        <v>944</v>
       </c>
       <c r="O348" t="s">
         <v>583</v>
@@ -18595,20 +18774,23 @@
       <c r="G349" t="s">
         <v>569</v>
       </c>
+      <c r="H349">
+        <v>0</v>
+      </c>
       <c r="J349" t="s">
-        <v>935</v>
+        <v>945</v>
       </c>
       <c r="K349" t="s">
         <v>571</v>
       </c>
       <c r="N349" t="s">
-        <v>936</v>
+        <v>946</v>
       </c>
       <c r="O349" t="s">
         <v>571</v>
       </c>
       <c r="R349" t="s">
-        <v>937</v>
+        <v>947</v>
       </c>
       <c r="V349" t="s">
         <v>30</v>
@@ -18639,6 +18821,9 @@
       <c r="G350" t="s">
         <v>583</v>
       </c>
+      <c r="H350" t="s">
+        <v>844</v>
+      </c>
       <c r="J350" t="s">
         <v>27</v>
       </c>
@@ -18646,13 +18831,13 @@
         <v>571</v>
       </c>
       <c r="N350" t="s">
-        <v>938</v>
+        <v>948</v>
       </c>
       <c r="O350" t="s">
         <v>574</v>
       </c>
       <c r="R350" t="s">
-        <v>939</v>
+        <v>949</v>
       </c>
       <c r="V350" t="s">
         <v>30</v>
@@ -18683,8 +18868,14 @@
       <c r="G351" t="s">
         <v>571</v>
       </c>
+      <c r="H351">
+        <v>0.25</v>
+      </c>
+      <c r="I351" t="s">
+        <v>950</v>
+      </c>
       <c r="J351" t="s">
-        <v>940</v>
+        <v>951</v>
       </c>
       <c r="K351" t="s">
         <v>571</v>
@@ -18693,13 +18884,13 @@
         <v>0.25</v>
       </c>
       <c r="N351" t="s">
-        <v>941</v>
+        <v>952</v>
       </c>
       <c r="O351" t="s">
         <v>571</v>
       </c>
       <c r="R351" t="s">
-        <v>942</v>
+        <v>953</v>
       </c>
       <c r="V351" t="s">
         <v>30</v>
@@ -18734,7 +18925,7 @@
         <v>0</v>
       </c>
       <c r="J352" t="s">
-        <v>943</v>
+        <v>954</v>
       </c>
       <c r="K352" t="s">
         <v>571</v>
@@ -18743,7 +18934,7 @@
         <v>0.25</v>
       </c>
       <c r="N352" t="s">
-        <v>944</v>
+        <v>955</v>
       </c>
       <c r="O352" t="s">
         <v>571</v>
@@ -18752,7 +18943,7 @@
         <v>0.25</v>
       </c>
       <c r="R352" t="s">
-        <v>945</v>
+        <v>956</v>
       </c>
       <c r="V352" t="s">
         <v>30</v>
@@ -18787,7 +18978,7 @@
         <v>0</v>
       </c>
       <c r="J353" t="s">
-        <v>946</v>
+        <v>957</v>
       </c>
       <c r="K353" t="s">
         <v>571</v>
@@ -18796,7 +18987,7 @@
         <v>0.25</v>
       </c>
       <c r="N353" t="s">
-        <v>947</v>
+        <v>958</v>
       </c>
       <c r="O353" t="s">
         <v>571</v>
@@ -18805,7 +18996,7 @@
         <v>0.5</v>
       </c>
       <c r="R353" t="s">
-        <v>948</v>
+        <v>959</v>
       </c>
       <c r="V353" t="s">
         <v>30</v>
@@ -18840,7 +19031,7 @@
         <v>0</v>
       </c>
       <c r="J354" t="s">
-        <v>949</v>
+        <v>960</v>
       </c>
       <c r="K354" t="s">
         <v>571</v>
@@ -18849,7 +19040,7 @@
         <v>0.25</v>
       </c>
       <c r="N354" t="s">
-        <v>950</v>
+        <v>961</v>
       </c>
       <c r="O354" t="s">
         <v>571</v>
@@ -18858,7 +19049,7 @@
         <v>0.5</v>
       </c>
       <c r="R354" t="s">
-        <v>951</v>
+        <v>962</v>
       </c>
       <c r="V354" t="s">
         <v>30</v>
@@ -18893,7 +19084,7 @@
         <v>0</v>
       </c>
       <c r="J355" t="s">
-        <v>952</v>
+        <v>963</v>
       </c>
       <c r="K355" t="s">
         <v>569</v>
@@ -18902,7 +19093,7 @@
         <v>0</v>
       </c>
       <c r="N355" t="s">
-        <v>953</v>
+        <v>964</v>
       </c>
       <c r="O355" t="s">
         <v>571</v>
@@ -18911,10 +19102,10 @@
         <v>0.25</v>
       </c>
       <c r="R355" t="s">
-        <v>954</v>
+        <v>965</v>
       </c>
       <c r="V355" t="s">
-        <v>955</v>
+        <v>966</v>
       </c>
       <c r="Z355" t="s">
         <v>31</v>
@@ -18946,7 +19137,7 @@
         <v>0</v>
       </c>
       <c r="J356" t="s">
-        <v>956</v>
+        <v>967</v>
       </c>
       <c r="K356" t="s">
         <v>574</v>
@@ -18955,7 +19146,7 @@
         <v>574</v>
       </c>
       <c r="N356" t="s">
-        <v>957</v>
+        <v>968</v>
       </c>
       <c r="O356" t="s">
         <v>571</v>
@@ -18964,7 +19155,7 @@
         <v>0.25</v>
       </c>
       <c r="R356" t="s">
-        <v>958</v>
+        <v>969</v>
       </c>
       <c r="V356" t="s">
         <v>30</v>
@@ -18999,7 +19190,7 @@
         <v>0</v>
       </c>
       <c r="J357" t="s">
-        <v>959</v>
+        <v>970</v>
       </c>
       <c r="K357" t="s">
         <v>569</v>
@@ -19008,7 +19199,7 @@
         <v>0</v>
       </c>
       <c r="N357" t="s">
-        <v>960</v>
+        <v>971</v>
       </c>
       <c r="O357" t="s">
         <v>571</v>
@@ -19017,7 +19208,7 @@
         <v>0.25</v>
       </c>
       <c r="R357" t="s">
-        <v>961</v>
+        <v>972</v>
       </c>
       <c r="V357" t="s">
         <v>30</v>
@@ -19052,7 +19243,7 @@
         <v>0</v>
       </c>
       <c r="J358" t="s">
-        <v>962</v>
+        <v>973</v>
       </c>
       <c r="K358" t="s">
         <v>569</v>
@@ -19061,7 +19252,7 @@
         <v>0</v>
       </c>
       <c r="N358" t="s">
-        <v>963</v>
+        <v>974</v>
       </c>
       <c r="O358" t="s">
         <v>571</v>
@@ -19070,7 +19261,7 @@
         <v>0.25</v>
       </c>
       <c r="R358" t="s">
-        <v>964</v>
+        <v>975</v>
       </c>
       <c r="V358" t="s">
         <v>30</v>
@@ -19105,7 +19296,7 @@
         <v>0</v>
       </c>
       <c r="J359" t="s">
-        <v>965</v>
+        <v>976</v>
       </c>
       <c r="K359" t="s">
         <v>569</v>
@@ -19114,7 +19305,7 @@
         <v>0</v>
       </c>
       <c r="N359" t="s">
-        <v>966</v>
+        <v>977</v>
       </c>
       <c r="O359" t="s">
         <v>571</v>
@@ -19123,7 +19314,7 @@
         <v>0.25</v>
       </c>
       <c r="R359" t="s">
-        <v>967</v>
+        <v>978</v>
       </c>
       <c r="V359" t="s">
         <v>30</v>
@@ -19158,7 +19349,7 @@
         <v>-0.25</v>
       </c>
       <c r="J360" t="s">
-        <v>968</v>
+        <v>979</v>
       </c>
       <c r="K360" t="s">
         <v>569</v>
@@ -19167,7 +19358,7 @@
         <v>0</v>
       </c>
       <c r="N360" t="s">
-        <v>969</v>
+        <v>980</v>
       </c>
       <c r="O360" t="s">
         <v>571</v>
@@ -19176,7 +19367,7 @@
         <v>0.25</v>
       </c>
       <c r="R360" t="s">
-        <v>970</v>
+        <v>981</v>
       </c>
       <c r="V360" t="s">
         <v>30</v>
@@ -19211,7 +19402,7 @@
         <v>-0.25</v>
       </c>
       <c r="J361" t="s">
-        <v>971</v>
+        <v>982</v>
       </c>
       <c r="K361" t="s">
         <v>569</v>
@@ -19220,7 +19411,7 @@
         <v>0</v>
       </c>
       <c r="N361" t="s">
-        <v>972</v>
+        <v>983</v>
       </c>
       <c r="O361" t="s">
         <v>571</v>
@@ -19229,7 +19420,7 @@
         <v>0.25</v>
       </c>
       <c r="R361" t="s">
-        <v>973</v>
+        <v>984</v>
       </c>
       <c r="V361" t="s">
         <v>30</v>
@@ -19264,7 +19455,7 @@
         <v>-0.25</v>
       </c>
       <c r="J362" t="s">
-        <v>974</v>
+        <v>985</v>
       </c>
       <c r="K362" t="s">
         <v>569</v>
@@ -19273,7 +19464,7 @@
         <v>0</v>
       </c>
       <c r="N362" t="s">
-        <v>975</v>
+        <v>986</v>
       </c>
       <c r="O362" t="s">
         <v>571</v>
@@ -19282,7 +19473,7 @@
         <v>0.25</v>
       </c>
       <c r="R362" t="s">
-        <v>976</v>
+        <v>987</v>
       </c>
       <c r="V362" t="s">
         <v>30</v>
@@ -19317,7 +19508,7 @@
         <v>-0.25</v>
       </c>
       <c r="J363" t="s">
-        <v>977</v>
+        <v>988</v>
       </c>
       <c r="K363" t="s">
         <v>569</v>
@@ -19326,7 +19517,7 @@
         <v>0</v>
       </c>
       <c r="N363" t="s">
-        <v>978</v>
+        <v>989</v>
       </c>
       <c r="O363" t="s">
         <v>571</v>
@@ -19335,7 +19526,7 @@
         <v>0.25</v>
       </c>
       <c r="R363" t="s">
-        <v>979</v>
+        <v>990</v>
       </c>
       <c r="V363" t="s">
         <v>30</v>
@@ -19370,7 +19561,7 @@
         <v>-0.5</v>
       </c>
       <c r="J364" t="s">
-        <v>980</v>
+        <v>991</v>
       </c>
       <c r="K364" t="s">
         <v>567</v>
@@ -19379,7 +19570,7 @@
         <v>-0.5</v>
       </c>
       <c r="N364" t="s">
-        <v>981</v>
+        <v>992</v>
       </c>
       <c r="O364" t="s">
         <v>567</v>
@@ -19388,10 +19579,10 @@
         <v>-0.25</v>
       </c>
       <c r="R364" t="s">
-        <v>982</v>
+        <v>993</v>
       </c>
       <c r="V364" t="s">
-        <v>983</v>
+        <v>994</v>
       </c>
       <c r="Z364" t="s">
         <v>31</v>
@@ -19423,16 +19614,16 @@
         <v>-0.25</v>
       </c>
       <c r="J365" t="s">
-        <v>984</v>
+        <v>995</v>
       </c>
       <c r="K365" t="s">
-        <v>985</v>
+        <v>996</v>
       </c>
       <c r="L365" t="s">
         <v>574</v>
       </c>
       <c r="N365" t="s">
-        <v>986</v>
+        <v>997</v>
       </c>
       <c r="O365" t="s">
         <v>569</v>
@@ -19441,7 +19632,7 @@
         <v>0</v>
       </c>
       <c r="R365" t="s">
-        <v>987</v>
+        <v>998</v>
       </c>
       <c r="V365" t="s">
         <v>30</v>
@@ -19476,7 +19667,7 @@
         <v>-0.5</v>
       </c>
       <c r="J366" t="s">
-        <v>988</v>
+        <v>999</v>
       </c>
       <c r="K366" t="s">
         <v>567</v>
@@ -19485,7 +19676,7 @@
         <v>-0.5</v>
       </c>
       <c r="N366" t="s">
-        <v>989</v>
+        <v>1000</v>
       </c>
       <c r="O366" t="s">
         <v>569</v>
@@ -19494,7 +19685,7 @@
         <v>0</v>
       </c>
       <c r="R366" t="s">
-        <v>990</v>
+        <v>1001</v>
       </c>
       <c r="V366" t="s">
         <v>30</v>
@@ -19529,7 +19720,7 @@
         <v>-0.75</v>
       </c>
       <c r="J367" t="s">
-        <v>991</v>
+        <v>1002</v>
       </c>
       <c r="K367" t="s">
         <v>567</v>
@@ -19538,7 +19729,7 @@
         <v>-0.5</v>
       </c>
       <c r="N367" t="s">
-        <v>992</v>
+        <v>1003</v>
       </c>
       <c r="O367" t="s">
         <v>567</v>
@@ -19547,10 +19738,10 @@
         <v>-0.25</v>
       </c>
       <c r="R367" t="s">
-        <v>993</v>
+        <v>1004</v>
       </c>
       <c r="V367" t="s">
-        <v>994</v>
+        <v>1005</v>
       </c>
       <c r="Z367" t="s">
         <v>31</v>
@@ -19582,7 +19773,7 @@
         <v>-0.75</v>
       </c>
       <c r="J368" t="s">
-        <v>995</v>
+        <v>1006</v>
       </c>
       <c r="K368" t="s">
         <v>567</v>
@@ -19591,7 +19782,7 @@
         <v>-0.5</v>
       </c>
       <c r="N368" t="s">
-        <v>996</v>
+        <v>1007</v>
       </c>
       <c r="O368" t="s">
         <v>567</v>
@@ -19600,10 +19791,10 @@
         <v>-0.25</v>
       </c>
       <c r="R368" t="s">
-        <v>997</v>
+        <v>1008</v>
       </c>
       <c r="V368" t="s">
-        <v>998</v>
+        <v>1009</v>
       </c>
       <c r="Z368" t="s">
         <v>31</v>
@@ -19635,7 +19826,7 @@
         <v>-0.5</v>
       </c>
       <c r="J369" t="s">
-        <v>999</v>
+        <v>1010</v>
       </c>
       <c r="K369" t="s">
         <v>567</v>
@@ -19644,7 +19835,7 @@
         <v>-0.25</v>
       </c>
       <c r="N369" t="s">
-        <v>1000</v>
+        <v>1011</v>
       </c>
       <c r="O369" t="s">
         <v>569</v>
@@ -19653,7 +19844,7 @@
         <v>0</v>
       </c>
       <c r="R369" t="s">
-        <v>1001</v>
+        <v>1012</v>
       </c>
       <c r="V369" t="s">
         <v>30</v>
@@ -19688,7 +19879,7 @@
         <v>-0.25</v>
       </c>
       <c r="J370" t="s">
-        <v>1002</v>
+        <v>1013</v>
       </c>
       <c r="K370" t="s">
         <v>569</v>
@@ -19697,7 +19888,7 @@
         <v>0</v>
       </c>
       <c r="N370" t="s">
-        <v>1003</v>
+        <v>1014</v>
       </c>
       <c r="O370" t="s">
         <v>571</v>
@@ -19706,7 +19897,7 @@
         <v>0.25</v>
       </c>
       <c r="R370" t="s">
-        <v>1004</v>
+        <v>1015</v>
       </c>
       <c r="V370" t="s">
         <v>30</v>
@@ -19747,7 +19938,7 @@
         <v>0</v>
       </c>
       <c r="N371" t="s">
-        <v>1005</v>
+        <v>1016</v>
       </c>
       <c r="O371" t="s">
         <v>571</v>
@@ -19756,7 +19947,7 @@
         <v>0.25</v>
       </c>
       <c r="R371" t="s">
-        <v>1006</v>
+        <v>1017</v>
       </c>
       <c r="V371" t="s">
         <v>30</v>
@@ -19791,7 +19982,7 @@
         <v>0</v>
       </c>
       <c r="J372" t="s">
-        <v>1007</v>
+        <v>1018</v>
       </c>
       <c r="K372" t="s">
         <v>569</v>
@@ -19800,7 +19991,7 @@
         <v>0</v>
       </c>
       <c r="N372" t="s">
-        <v>1008</v>
+        <v>1019</v>
       </c>
       <c r="O372" t="s">
         <v>571</v>
@@ -19809,7 +20000,7 @@
         <v>0.25</v>
       </c>
       <c r="R372" t="s">
-        <v>1009</v>
+        <v>1020</v>
       </c>
       <c r="V372" t="s">
         <v>30</v>
@@ -19844,7 +20035,7 @@
         <v>-0.5</v>
       </c>
       <c r="J373" t="s">
-        <v>1010</v>
+        <v>1021</v>
       </c>
       <c r="K373" t="s">
         <v>567</v>
@@ -19853,7 +20044,7 @@
         <v>-0.25</v>
       </c>
       <c r="N373" t="s">
-        <v>1011</v>
+        <v>1022</v>
       </c>
       <c r="O373" t="s">
         <v>569</v>
@@ -19862,7 +20053,7 @@
         <v>0</v>
       </c>
       <c r="R373" t="s">
-        <v>1012</v>
+        <v>1023</v>
       </c>
       <c r="V373" t="s">
         <v>30</v>
@@ -19897,7 +20088,7 @@
         <v>-1</v>
       </c>
       <c r="J374" t="s">
-        <v>1013</v>
+        <v>1024</v>
       </c>
       <c r="K374" t="s">
         <v>567</v>
@@ -19906,7 +20097,7 @@
         <v>-0.25</v>
       </c>
       <c r="N374" t="s">
-        <v>1014</v>
+        <v>1025</v>
       </c>
       <c r="O374" t="s">
         <v>567</v>
@@ -19915,10 +20106,10 @@
         <v>-0.5</v>
       </c>
       <c r="R374" t="s">
-        <v>1015</v>
+        <v>1026</v>
       </c>
       <c r="V374" t="s">
-        <v>1016</v>
+        <v>1027</v>
       </c>
       <c r="Z374" t="s">
         <v>31</v>
@@ -19947,10 +20138,10 @@
         <v>567</v>
       </c>
       <c r="H375" t="s">
-        <v>1017</v>
+        <v>1028</v>
       </c>
       <c r="J375" t="s">
-        <v>1018</v>
+        <v>1029</v>
       </c>
       <c r="K375" t="s">
         <v>567</v>
@@ -19959,7 +20150,7 @@
         <v>574</v>
       </c>
       <c r="N375" t="s">
-        <v>1019</v>
+        <v>1030</v>
       </c>
       <c r="O375" t="s">
         <v>569</v>
@@ -19968,7 +20159,7 @@
         <v>0</v>
       </c>
       <c r="R375" t="s">
-        <v>1020</v>
+        <v>1031</v>
       </c>
       <c r="V375" t="s">
         <v>30</v>
@@ -20000,19 +20191,19 @@
         <v>567</v>
       </c>
       <c r="H376" t="s">
-        <v>1021</v>
+        <v>1032</v>
       </c>
       <c r="J376" t="s">
-        <v>1022</v>
+        <v>1033</v>
       </c>
       <c r="K376" t="s">
         <v>567</v>
       </c>
       <c r="L376" t="s">
-        <v>1023</v>
+        <v>1034</v>
       </c>
       <c r="N376" t="s">
-        <v>1024</v>
+        <v>1035</v>
       </c>
       <c r="O376" t="s">
         <v>569</v>
@@ -20021,7 +20212,7 @@
         <v>0</v>
       </c>
       <c r="R376" t="s">
-        <v>1025</v>
+        <v>1036</v>
       </c>
       <c r="V376" t="s">
         <v>30</v>

</xml_diff>